<commit_message>
copying over updated and added files to new clone
</commit_message>
<xml_diff>
--- a/Stochastic_engine/Synthetic_wind_power/cap_by_month.xlsx
+++ b/Stochastic_engine/Synthetic_wind_power/cap_by_month.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdkern\Desktop\PostDoc\python files\CAPOW\Stochastic_inputs\Wind_Solar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jawessel\Documents\GitHub\CAPOW_jaw\Stochastic_engine\Synthetic_wind_power\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16598" windowHeight="6555" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16600" windowHeight="6560" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="wind" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>Month</t>
   </si>
@@ -99,7 +99,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -111,6 +111,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -399,15 +402,15 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.06640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.73046875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.73046875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.73046875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7265625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -421,7 +424,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="17.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -436,7 +439,7 @@
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -450,7 +453,7 @@
         <v>3569.5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -464,7 +467,7 @@
         <v>3742</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -478,7 +481,7 @@
         <v>3742</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -492,7 +495,7 @@
         <v>4012</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -506,7 +509,7 @@
         <v>4012</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -520,7 +523,7 @@
         <v>4012</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -534,7 +537,7 @@
         <v>4012</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -548,7 +551,7 @@
         <v>4012</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -562,7 +565,7 @@
         <v>4012</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -576,7 +579,7 @@
         <v>4012</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -590,7 +593,7 @@
         <v>4012</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>1</v>
       </c>
@@ -604,7 +607,7 @@
         <v>4112</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>2</v>
       </c>
@@ -618,7 +621,7 @@
         <v>4580.2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>3</v>
       </c>
@@ -632,7 +635,7 @@
         <v>4629.2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>4</v>
       </c>
@@ -646,7 +649,7 @@
         <v>4764.2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>5</v>
       </c>
@@ -660,7 +663,7 @@
         <v>4892</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>6</v>
       </c>
@@ -674,7 +677,7 @@
         <v>5042</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>7</v>
       </c>
@@ -688,7 +691,7 @@
         <v>5042</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>8</v>
       </c>
@@ -702,7 +705,7 @@
         <v>5042</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>9</v>
       </c>
@@ -716,7 +719,7 @@
         <v>5042</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>10</v>
       </c>
@@ -730,7 +733,7 @@
         <v>5042</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>11</v>
       </c>
@@ -744,7 +747,7 @@
         <v>5042</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>12</v>
       </c>
@@ -758,7 +761,7 @@
         <v>5204</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>1</v>
       </c>
@@ -772,7 +775,7 @@
         <v>5876.5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>2</v>
       </c>
@@ -786,7 +789,7 @@
         <v>5876.5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>3</v>
       </c>
@@ -800,7 +803,7 @@
         <v>5876.5</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>4</v>
       </c>
@@ -814,7 +817,7 @@
         <v>5876.5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>5</v>
       </c>
@@ -828,7 +831,7 @@
         <v>5876.5</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>6</v>
       </c>
@@ -842,7 +845,7 @@
         <v>5876.5</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>7</v>
       </c>
@@ -856,7 +859,7 @@
         <v>5876.5</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>8</v>
       </c>
@@ -870,7 +873,7 @@
         <v>6141.9</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>9</v>
       </c>
@@ -884,7 +887,7 @@
         <v>6141.9</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>10</v>
       </c>
@@ -898,7 +901,7 @@
         <v>6141.9</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>11</v>
       </c>
@@ -912,7 +915,7 @@
         <v>6141.9</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>12</v>
       </c>
@@ -926,7 +929,7 @@
         <v>6141.9</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>1</v>
       </c>
@@ -940,7 +943,7 @@
         <v>6141.9</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>2</v>
       </c>
@@ -954,7 +957,7 @@
         <v>6141.9</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>3</v>
       </c>
@@ -968,7 +971,7 @@
         <v>6146.0999999999995</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>4</v>
       </c>
@@ -982,7 +985,7 @@
         <v>6146.0999999999995</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>5</v>
       </c>
@@ -996,7 +999,7 @@
         <v>6146.0999999999995</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>6</v>
       </c>
@@ -1010,7 +1013,7 @@
         <v>6146.0999999999995</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>7</v>
       </c>
@@ -1024,7 +1027,7 @@
         <v>6153.5599999999995</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
         <v>8</v>
       </c>
@@ -1038,7 +1041,7 @@
         <v>6153.5599999999995</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
         <v>9</v>
       </c>
@@ -1052,7 +1055,7 @@
         <v>6153.5599999999995</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
         <v>10</v>
       </c>
@@ -1066,7 +1069,7 @@
         <v>6153.5599999999995</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
         <v>11</v>
       </c>
@@ -1080,7 +1083,7 @@
         <v>6153.5599999999995</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
         <v>12</v>
       </c>
@@ -1094,7 +1097,7 @@
         <v>6153.5599999999995</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
         <v>1</v>
       </c>
@@ -1108,7 +1111,7 @@
         <v>6200.6799999999994</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
         <v>2</v>
       </c>
@@ -1122,7 +1125,7 @@
         <v>6311.4599999999991</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
         <v>3</v>
       </c>
@@ -1136,7 +1139,7 @@
         <v>6311.4599999999991</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="2">
         <v>4</v>
       </c>
@@ -1150,7 +1153,7 @@
         <v>6311.4599999999991</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="2">
         <v>5</v>
       </c>
@@ -1164,7 +1167,7 @@
         <v>6311.4599999999991</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="2">
         <v>6</v>
       </c>
@@ -1178,7 +1181,7 @@
         <v>6311.4599999999991</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="2">
         <v>7</v>
       </c>
@@ -1192,7 +1195,7 @@
         <v>6410.4599999999991</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="2">
         <v>8</v>
       </c>
@@ -1206,7 +1209,7 @@
         <v>6422.1599999999989</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="2">
         <v>9</v>
       </c>
@@ -1220,7 +1223,7 @@
         <v>6422.1599999999989</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="2">
         <v>10</v>
       </c>
@@ -1234,7 +1237,7 @@
         <v>6422.1599999999989</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="2">
         <v>11</v>
       </c>
@@ -1248,7 +1251,7 @@
         <v>6442.1599999999989</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="2">
         <v>12</v>
       </c>
@@ -1262,7 +1265,7 @@
         <v>6489.4199999999992</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="2">
         <v>1</v>
       </c>
@@ -1276,7 +1279,7 @@
         <v>6489.4199999999992</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="2">
         <v>2</v>
       </c>
@@ -1290,7 +1293,7 @@
         <v>6501.3199999999988</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="2">
         <v>3</v>
       </c>
@@ -1304,7 +1307,7 @@
         <v>6501.3199999999988</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="2">
         <v>4</v>
       </c>
@@ -1318,7 +1321,7 @@
         <v>6501.3199999999988</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="2">
         <v>5</v>
       </c>
@@ -1332,7 +1335,7 @@
         <v>6501.3199999999988</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="2">
         <v>6</v>
       </c>
@@ -1346,7 +1349,7 @@
         <v>6501.3199999999988</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="2">
         <v>7</v>
       </c>
@@ -1360,7 +1363,7 @@
         <v>6501.3199999999988</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="2">
         <v>8</v>
       </c>
@@ -1374,7 +1377,7 @@
         <v>6501.3199999999988</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="2">
         <v>9</v>
       </c>
@@ -1388,7 +1391,7 @@
         <v>6501.3199999999988</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="2">
         <v>10</v>
       </c>
@@ -1402,7 +1405,7 @@
         <v>6501.3199999999988</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="2">
         <v>11</v>
       </c>
@@ -1416,7 +1419,7 @@
         <v>6501.3199999999988</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="2">
         <v>12</v>
       </c>
@@ -1430,7 +1433,7 @@
         <v>6501.3199999999988</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" s="2">
         <v>1</v>
       </c>
@@ -1444,7 +1447,7 @@
         <v>6501.3199999999988</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="2">
         <v>2</v>
       </c>
@@ -1458,7 +1461,7 @@
         <v>6501.3199999999988</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="2">
         <v>3</v>
       </c>
@@ -1472,7 +1475,7 @@
         <v>6501.3199999999988</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" s="2">
         <v>4</v>
       </c>
@@ -1486,7 +1489,7 @@
         <v>6501.3199999999988</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="2">
         <v>5</v>
       </c>
@@ -1500,7 +1503,7 @@
         <v>6501.3199999999988</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="2">
         <v>6</v>
       </c>
@@ -1514,7 +1517,7 @@
         <v>6501.3199999999988</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" s="2">
         <v>7</v>
       </c>
@@ -1528,7 +1531,7 @@
         <v>6501.3199999999988</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" s="2">
         <v>8</v>
       </c>
@@ -1542,7 +1545,7 @@
         <v>6501.3199999999988</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" s="2">
         <v>9</v>
       </c>
@@ -1556,7 +1559,7 @@
         <v>6501.3199999999988</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" s="2">
         <v>10</v>
       </c>
@@ -1570,7 +1573,7 @@
         <v>6501.3199999999988</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" s="2">
         <v>11</v>
       </c>
@@ -1584,7 +1587,7 @@
         <v>6547.32</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" s="2">
         <v>12</v>
       </c>
@@ -1605,20 +1608,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C85"/>
+  <dimension ref="A1:D85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.06640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1628,8 +1631,11 @@
       <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1639,8 +1645,11 @@
       <c r="C2" s="4">
         <v>703.51</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D2" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1650,8 +1659,11 @@
       <c r="C3" s="4">
         <v>703.51</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D3" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1661,8 +1673,11 @@
       <c r="C4" s="4">
         <v>704.51</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D4" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1672,8 +1687,11 @@
       <c r="C5" s="4">
         <v>704.51</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D5" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1683,8 +1701,11 @@
       <c r="C6" s="4">
         <v>704.51</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D6" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1694,8 +1715,11 @@
       <c r="C7" s="4">
         <v>704.51</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D7" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1705,8 +1729,11 @@
       <c r="C8" s="4">
         <v>704.51</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D8" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1716,8 +1743,11 @@
       <c r="C9" s="4">
         <v>708.51</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D9" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1727,8 +1757,11 @@
       <c r="C10" s="4">
         <v>759.01</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D10" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1738,8 +1771,11 @@
       <c r="C11" s="4">
         <v>804.01</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D11" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1749,8 +1785,11 @@
       <c r="C12" s="4">
         <v>819.01</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D12" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1760,8 +1799,11 @@
       <c r="C13" s="4">
         <v>819.01</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D13" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>1</v>
       </c>
@@ -1771,8 +1813,11 @@
       <c r="C14" s="4">
         <v>819.01</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D14" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>2</v>
       </c>
@@ -1782,8 +1827,11 @@
       <c r="C15" s="4">
         <v>819.01</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D15" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>3</v>
       </c>
@@ -1793,8 +1841,11 @@
       <c r="C16" s="4">
         <v>820.18</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D16" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>4</v>
       </c>
@@ -1804,8 +1855,11 @@
       <c r="C17" s="4">
         <v>825.82999999999993</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D17" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>5</v>
       </c>
@@ -1815,8 +1869,11 @@
       <c r="C18" s="4">
         <v>825.82999999999993</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D18" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>6</v>
       </c>
@@ -1826,8 +1883,11 @@
       <c r="C19" s="4">
         <v>829.82999999999993</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D19" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>7</v>
       </c>
@@ -1837,8 +1897,11 @@
       <c r="C20" s="4">
         <v>829.82999999999993</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D20" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>8</v>
       </c>
@@ -1848,8 +1911,11 @@
       <c r="C21" s="4">
         <v>868.82999999999993</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D21" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>9</v>
       </c>
@@ -1859,8 +1925,11 @@
       <c r="C22" s="4">
         <v>888.82999999999993</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D22" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>10</v>
       </c>
@@ -1870,8 +1939,11 @@
       <c r="C23" s="4">
         <v>888.82999999999993</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D23" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>11</v>
       </c>
@@ -1881,8 +1953,11 @@
       <c r="C24" s="4">
         <v>892.94999999999993</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D24" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>12</v>
       </c>
@@ -1892,8 +1967,11 @@
       <c r="C25" s="4">
         <v>905.94999999999993</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D25" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>1</v>
       </c>
@@ -1903,8 +1981,11 @@
       <c r="C26" s="4">
         <v>955.44999999999993</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D26" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>2</v>
       </c>
@@ -1914,8 +1995,11 @@
       <c r="C27" s="4">
         <v>1028.4499999999998</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D27" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>3</v>
       </c>
@@ -1925,8 +2009,11 @@
       <c r="C28" s="4">
         <v>1054.4499999999998</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D28" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>4</v>
       </c>
@@ -1936,8 +2023,11 @@
       <c r="C29" s="4">
         <v>1166.9499999999998</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D29" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>5</v>
       </c>
@@ -1947,8 +2037,11 @@
       <c r="C30" s="4">
         <v>1167.9499999999998</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D30" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>6</v>
       </c>
@@ -1958,8 +2051,11 @@
       <c r="C31" s="4">
         <v>1188.9499999999998</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D31" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>7</v>
       </c>
@@ -1969,8 +2065,11 @@
       <c r="C32" s="4">
         <v>1275.4499999999998</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D32" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>8</v>
       </c>
@@ -1980,8 +2079,11 @@
       <c r="C33" s="4">
         <v>1277.4499999999998</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D33" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>9</v>
       </c>
@@ -1991,8 +2093,11 @@
       <c r="C34" s="4">
         <v>1305.9499999999998</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D34" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>10</v>
       </c>
@@ -2002,8 +2107,11 @@
       <c r="C35" s="4">
         <v>1325.9499999999998</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D35" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>11</v>
       </c>
@@ -2013,8 +2121,11 @@
       <c r="C36" s="4">
         <v>1942.9499999999998</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D36" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>12</v>
       </c>
@@ -2024,8 +2135,11 @@
       <c r="C37" s="4">
         <v>2483.9499999999998</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D37" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>1</v>
       </c>
@@ -2035,8 +2149,11 @@
       <c r="C38" s="4">
         <v>3113.95</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D38" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>2</v>
       </c>
@@ -2046,8 +2163,11 @@
       <c r="C39" s="4">
         <v>3115.45</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D39" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>3</v>
       </c>
@@ -2057,8 +2177,11 @@
       <c r="C40" s="4">
         <v>3338.95</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D40" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>4</v>
       </c>
@@ -2068,8 +2191,11 @@
       <c r="C41" s="4">
         <v>3339.95</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D41" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>5</v>
       </c>
@@ -2079,8 +2205,11 @@
       <c r="C42" s="4">
         <v>3363.95</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D42" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>6</v>
       </c>
@@ -2090,8 +2219,11 @@
       <c r="C43" s="4">
         <v>3928.2</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D43" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>7</v>
       </c>
@@ -2101,8 +2233,11 @@
       <c r="C44" s="4">
         <v>3928.2</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D44" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
         <v>8</v>
       </c>
@@ -2112,8 +2247,11 @@
       <c r="C45" s="4">
         <v>4055.2</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D45" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
         <v>9</v>
       </c>
@@ -2123,8 +2261,11 @@
       <c r="C46" s="4">
         <v>4102.3</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D46" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
         <v>10</v>
       </c>
@@ -2134,8 +2275,11 @@
       <c r="C47" s="4">
         <v>4122.05</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D47" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
         <v>11</v>
       </c>
@@ -2145,8 +2289,11 @@
       <c r="C48" s="4">
         <v>4672.05</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D48" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
         <v>12</v>
       </c>
@@ -2156,8 +2303,11 @@
       <c r="C49" s="4">
         <v>5955.9000000000005</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D49" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
         <v>1</v>
       </c>
@@ -2167,8 +2317,11 @@
       <c r="C50" s="4">
         <v>6100.9000000000005</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D50" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
         <v>2</v>
       </c>
@@ -2178,8 +2331,11 @@
       <c r="C51" s="4">
         <v>6145.9000000000005</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D51" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
         <v>3</v>
       </c>
@@ -2189,8 +2345,11 @@
       <c r="C52" s="4">
         <v>6165.9000000000005</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D52" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="2">
         <v>4</v>
       </c>
@@ -2200,8 +2359,11 @@
       <c r="C53" s="4">
         <v>6208.1100000000006</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D53" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="2">
         <v>5</v>
       </c>
@@ -2211,8 +2373,11 @@
       <c r="C54" s="4">
         <v>6246.09</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D54" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="2">
         <v>6</v>
       </c>
@@ -2222,8 +2387,11 @@
       <c r="C55" s="4">
         <v>6359.84</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D55" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="2">
         <v>7</v>
       </c>
@@ -2233,8 +2401,11 @@
       <c r="C56" s="4">
         <v>6732.84</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D56" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="2">
         <v>8</v>
       </c>
@@ -2244,8 +2415,11 @@
       <c r="C57" s="4">
         <v>6764.24</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D57" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="2">
         <v>9</v>
       </c>
@@ -2255,8 +2429,11 @@
       <c r="C58" s="4">
         <v>6954.24</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D58" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="2">
         <v>10</v>
       </c>
@@ -2266,8 +2443,11 @@
       <c r="C59" s="4">
         <v>6987.24</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D59" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="2">
         <v>11</v>
       </c>
@@ -2277,8 +2457,11 @@
       <c r="C60" s="4">
         <v>7030.0999999999995</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D60" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="2">
         <v>12</v>
       </c>
@@ -2288,8 +2471,11 @@
       <c r="C61" s="4">
         <v>7173.5999999999995</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D61" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="2">
         <v>1</v>
       </c>
@@ -2299,8 +2485,11 @@
       <c r="C62" s="4">
         <v>7292.11</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D62" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="2">
         <v>2</v>
       </c>
@@ -2310,8 +2499,11 @@
       <c r="C63" s="4">
         <v>7483.01</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D63" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="2">
         <v>3</v>
       </c>
@@ -2321,8 +2513,11 @@
       <c r="C64" s="4">
         <v>7523</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D64" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="2">
         <v>4</v>
       </c>
@@ -2332,8 +2527,11 @@
       <c r="C65" s="4">
         <v>7530</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D65" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="2">
         <v>5</v>
       </c>
@@ -2343,8 +2541,11 @@
       <c r="C66" s="4">
         <v>7720</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D66" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="2">
         <v>6</v>
       </c>
@@ -2354,8 +2555,11 @@
       <c r="C67" s="4">
         <v>7742</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D67" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="2">
         <v>7</v>
       </c>
@@ -2365,8 +2569,11 @@
       <c r="C68" s="4">
         <v>8322</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D68" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="2">
         <v>8</v>
       </c>
@@ -2376,8 +2583,11 @@
       <c r="C69" s="4">
         <v>8991.99</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D69" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="2">
         <v>9</v>
       </c>
@@ -2387,8 +2597,11 @@
       <c r="C70" s="4">
         <v>8991.99</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D70" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="2">
         <v>10</v>
       </c>
@@ -2398,8 +2611,11 @@
       <c r="C71" s="4">
         <v>9049.99</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D71" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="2">
         <v>11</v>
       </c>
@@ -2409,8 +2625,11 @@
       <c r="C72" s="4">
         <v>9589.99</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D72" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="2">
         <v>12</v>
       </c>
@@ -2420,8 +2639,11 @@
       <c r="C73" s="4">
         <v>9758.99</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D73" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" s="2">
         <v>1</v>
       </c>
@@ -2431,8 +2653,11 @@
       <c r="C74" s="4">
         <v>9916.32</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D74" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="2">
         <v>2</v>
       </c>
@@ -2442,8 +2667,11 @@
       <c r="C75" s="4">
         <v>9979.119999999999</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D75" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="2">
         <v>3</v>
       </c>
@@ -2453,8 +2681,11 @@
       <c r="C76" s="4">
         <v>10029.219999999998</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D76" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" s="2">
         <v>4</v>
       </c>
@@ -2464,8 +2695,11 @@
       <c r="C77" s="4">
         <v>10071.219999999998</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D77" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="2">
         <v>5</v>
       </c>
@@ -2475,8 +2709,11 @@
       <c r="C78" s="4">
         <v>10156.219999999998</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D78" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="2">
         <v>6</v>
       </c>
@@ -2486,8 +2723,11 @@
       <c r="C79" s="4">
         <v>10176.219999999998</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D79" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" s="2">
         <v>7</v>
       </c>
@@ -2497,8 +2737,11 @@
       <c r="C80" s="4">
         <v>10213.019999999997</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D80" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" s="2">
         <v>8</v>
       </c>
@@ -2508,8 +2751,11 @@
       <c r="C81" s="4">
         <v>10232.719999999998</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D81" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" s="2">
         <v>9</v>
       </c>
@@ -2519,8 +2765,11 @@
       <c r="C82" s="4">
         <v>10240.319999999996</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D82" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" s="2">
         <v>10</v>
       </c>
@@ -2530,8 +2779,11 @@
       <c r="C83" s="4">
         <v>10254.319999999996</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D83" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" s="2">
         <v>11</v>
       </c>
@@ -2541,8 +2793,11 @@
       <c r="C84" s="4">
         <v>10419.319999999996</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D84" s="5">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" s="2">
         <v>12</v>
       </c>
@@ -2551,6 +2806,9 @@
       </c>
       <c r="C85" s="4">
         <v>10589.319999999996</v>
+      </c>
+      <c r="D85" s="5">
+        <v>85.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>